<commit_message>
Agregado Generador de mapas y trayectoria
</commit_message>
<xml_diff>
--- a/mapfiles/template_mapsWAY.xlsx
+++ b/mapfiles/template_mapsWAY.xlsx
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S31" workbookViewId="0">
-      <selection activeCell="AI43" sqref="AI43"/>
+    <sheetView tabSelected="1" topLeftCell="S34" workbookViewId="0">
+      <selection activeCell="AG53" sqref="AG53:AI53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4664,9 +4664,6 @@
       <c r="C42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E42" s="1" t="s">
         <v>1</v>
       </c>
@@ -4691,13 +4688,13 @@
       <c r="L42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="N42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q42" s="1" t="s">
@@ -4716,7 +4713,7 @@
       </c>
       <c r="W42" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>15,13;-1</v>
       </c>
       <c r="X42" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4752,7 +4749,7 @@
       </c>
       <c r="AF42" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>15,4;-1</v>
       </c>
       <c r="AG42" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4764,7 +4761,7 @@
       </c>
       <c r="AI42" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>15,1;-1</v>
+        <v/>
       </c>
       <c r="AJ42" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4781,9 +4778,6 @@
       <c r="C43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E43" s="1" t="s">
         <v>1</v>
       </c>
@@ -4808,13 +4802,13 @@
       <c r="L43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="N43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q43" s="1" t="s">
@@ -4833,7 +4827,7 @@
       </c>
       <c r="W43" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>14,13;-1</v>
       </c>
       <c r="X43" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4869,7 +4863,7 @@
       </c>
       <c r="AF43" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>14,4;-1</v>
       </c>
       <c r="AG43" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4881,7 +4875,7 @@
       </c>
       <c r="AI43" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>14,1;-1</v>
+        <v/>
       </c>
       <c r="AJ43" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4898,6 +4892,39 @@
       <c r="C44" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="Q44" s="1" t="s">
         <v>1</v>
       </c>
@@ -4918,35 +4945,35 @@
       </c>
       <c r="X44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,12;-1</v>
+        <v/>
       </c>
       <c r="Y44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,11;-1</v>
+        <v/>
       </c>
       <c r="Z44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,10;-1</v>
+        <v/>
       </c>
       <c r="AA44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,9;-1</v>
+        <v/>
       </c>
       <c r="AB44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,8;-1</v>
+        <v/>
       </c>
       <c r="AC44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,7;-1</v>
+        <v/>
       </c>
       <c r="AD44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,6;-1</v>
+        <v/>
       </c>
       <c r="AE44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,5;-1</v>
+        <v/>
       </c>
       <c r="AF44" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4954,15 +4981,15 @@
       </c>
       <c r="AG44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,3;-1</v>
+        <v/>
       </c>
       <c r="AH44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,2;-1</v>
+        <v/>
       </c>
       <c r="AI44" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>13,1;-1</v>
+        <v/>
       </c>
       <c r="AJ44" s="1" t="str">
         <f t="shared" si="5"/>
@@ -4988,24 +5015,6 @@
       <c r="G45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="O45" s="1" t="s">
         <v>1</v>
       </c>
@@ -5044,19 +5053,19 @@
       </c>
       <c r="AA45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,9;-1</v>
       </c>
       <c r="AB45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,8;-1</v>
       </c>
       <c r="AC45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,7;-1</v>
       </c>
       <c r="AD45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,6;-1</v>
       </c>
       <c r="AE45" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5064,11 +5073,11 @@
       </c>
       <c r="AF45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,4;-1</v>
       </c>
       <c r="AG45" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>12,3;-1</v>
       </c>
       <c r="AH45" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5093,18 +5102,6 @@
       <c r="C46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="I46" s="1" t="s">
         <v>1</v>
       </c>
@@ -5114,10 +5111,10 @@
       <c r="K46" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="L46" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="M46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O46" s="1" t="s">
@@ -5146,19 +5143,19 @@
       </c>
       <c r="X46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>11,12;-1</v>
       </c>
       <c r="Y46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>11,11;-1</v>
       </c>
       <c r="Z46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>11,10;-1</v>
       </c>
       <c r="AA46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>11,9;-1</v>
       </c>
       <c r="AB46" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5174,7 +5171,7 @@
       </c>
       <c r="AE46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>11,5;-1</v>
+        <v/>
       </c>
       <c r="AF46" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5182,7 +5179,7 @@
       </c>
       <c r="AG46" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>11,3;-1</v>
       </c>
       <c r="AH46" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5207,16 +5204,28 @@
       <c r="C47" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D47" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="H47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O47" s="1" t="s">
@@ -5241,7 +5250,7 @@
       </c>
       <c r="W47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,13;-1</v>
+        <v/>
       </c>
       <c r="X47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5249,7 +5258,7 @@
       </c>
       <c r="Y47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>10,11;-1</v>
       </c>
       <c r="Z47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5257,23 +5266,23 @@
       </c>
       <c r="AA47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,9;-1</v>
+        <v/>
       </c>
       <c r="AB47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,8;-1</v>
+        <v/>
       </c>
       <c r="AC47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,7;-1</v>
+        <v/>
       </c>
       <c r="AD47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,6;-1</v>
+        <v/>
       </c>
       <c r="AE47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>10,5;-1</v>
+        <v/>
       </c>
       <c r="AF47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5281,7 +5290,7 @@
       </c>
       <c r="AG47" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>10,3;-1</v>
       </c>
       <c r="AH47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5306,12 +5315,12 @@
       <c r="C48" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D48" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G48" s="1" t="s">
         <v>1</v>
       </c>
@@ -5319,18 +5328,6 @@
         <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O48" s="1" t="s">
@@ -5355,7 +5352,7 @@
       </c>
       <c r="W48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>9,13;-1</v>
+        <v/>
       </c>
       <c r="X48" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5363,7 +5360,7 @@
       </c>
       <c r="Y48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9,11;-1</v>
       </c>
       <c r="Z48" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5379,11 +5376,11 @@
       </c>
       <c r="AC48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9,7;-1</v>
       </c>
       <c r="AD48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9,6;-1</v>
       </c>
       <c r="AE48" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5391,11 +5388,11 @@
       </c>
       <c r="AF48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9,4;-1</v>
       </c>
       <c r="AG48" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>9,3;-1</v>
       </c>
       <c r="AH48" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5420,12 +5417,12 @@
       <c r="C49" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D49" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G49" s="1" t="s">
         <v>1</v>
       </c>
@@ -5435,10 +5432,16 @@
       <c r="I49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="K49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O49" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P49" s="1" t="s">
@@ -5460,7 +5463,7 @@
       </c>
       <c r="W49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>8,13;-1</v>
+        <v/>
       </c>
       <c r="X49" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5468,7 +5471,7 @@
       </c>
       <c r="Y49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>8,11;-1</v>
       </c>
       <c r="Z49" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5484,7 +5487,7 @@
       </c>
       <c r="AC49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>8,7;-1</v>
       </c>
       <c r="AD49" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5492,19 +5495,19 @@
       </c>
       <c r="AE49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>8,5;-1</v>
+        <v/>
       </c>
       <c r="AF49" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(M49="O","",CONCATENATE(M9,";-1"))</f>
         <v>8,4;-1</v>
       </c>
       <c r="AG49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>8,3;-1</v>
+        <v/>
       </c>
       <c r="AH49" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>8,2;-1</v>
+        <v/>
       </c>
       <c r="AI49" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5525,12 +5528,12 @@
       <c r="C50" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D50" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G50" s="1" t="s">
         <v>1</v>
       </c>
@@ -5540,19 +5543,16 @@
       <c r="I50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="K50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M50" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="N50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P50" s="1" t="s">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="W50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>7,13;-1</v>
+        <v/>
       </c>
       <c r="X50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5582,7 +5582,7 @@
       </c>
       <c r="Y50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>7,11;-1</v>
       </c>
       <c r="Z50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="AC50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>7,7;-1</v>
       </c>
       <c r="AD50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5610,7 +5610,7 @@
       </c>
       <c r="AF50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>7,4;-1</v>
       </c>
       <c r="AG50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5618,7 +5618,7 @@
       </c>
       <c r="AH50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>7,2;-1</v>
+        <v/>
       </c>
       <c r="AI50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5639,7 +5639,19 @@
       <c r="C51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="D51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K51" s="1" t="s">
@@ -5648,10 +5660,10 @@
       <c r="L51" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="N51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P51" s="1" t="s">
@@ -5673,11 +5685,11 @@
       </c>
       <c r="W51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,13;-1</v>
+        <v/>
       </c>
       <c r="X51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,12;-1</v>
+        <v/>
       </c>
       <c r="Y51" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5685,19 +5697,19 @@
       </c>
       <c r="Z51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,10;-1</v>
+        <v/>
       </c>
       <c r="AA51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,9;-1</v>
+        <v/>
       </c>
       <c r="AB51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,8;-1</v>
+        <v/>
       </c>
       <c r="AC51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>6,7;-1</v>
       </c>
       <c r="AD51" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5709,7 +5721,7 @@
       </c>
       <c r="AF51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>6,4;-1</v>
       </c>
       <c r="AG51" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5717,7 +5729,7 @@
       </c>
       <c r="AH51" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>6,2;-1</v>
+        <v/>
       </c>
       <c r="AI51" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5744,19 +5756,25 @@
       <c r="E52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P52" s="1" t="s">
@@ -5786,7 +5804,7 @@
       </c>
       <c r="Y52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>5,11;-1</v>
       </c>
       <c r="Z52" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5798,11 +5816,11 @@
       </c>
       <c r="AB52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>5,8;-1</v>
+        <v/>
       </c>
       <c r="AC52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>5,7;-1</v>
       </c>
       <c r="AD52" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5810,7 +5828,7 @@
       </c>
       <c r="AE52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>5,5;-1</v>
+        <v/>
       </c>
       <c r="AF52" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5818,11 +5836,11 @@
       </c>
       <c r="AG52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>5,3;-1</v>
+        <v/>
       </c>
       <c r="AH52" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>5,2;-1</v>
+        <v/>
       </c>
       <c r="AI52" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5843,37 +5861,19 @@
       <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="Q53" s="1" t="s">
@@ -5892,15 +5892,15 @@
       </c>
       <c r="W53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,13;-1</v>
       </c>
       <c r="X53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,12;-1</v>
       </c>
       <c r="Y53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,11;-1</v>
       </c>
       <c r="Z53" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5912,11 +5912,11 @@
       </c>
       <c r="AB53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>4,8;-1</v>
+        <v/>
       </c>
       <c r="AC53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,7;-1</v>
       </c>
       <c r="AD53" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5924,23 +5924,23 @@
       </c>
       <c r="AE53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>4,5;-1</v>
+        <v/>
       </c>
       <c r="AF53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,4;-1</v>
       </c>
       <c r="AG53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,3;-1</v>
       </c>
       <c r="AH53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,2;-1</v>
       </c>
       <c r="AI53" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>4,1;-1</v>
       </c>
       <c r="AJ53" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5957,9 +5957,6 @@
       <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E54" s="1" t="s">
         <v>1</v>
       </c>
@@ -5972,10 +5969,13 @@
       <c r="H54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M54" s="1" t="s">
@@ -6006,7 +6006,7 @@
       </c>
       <c r="W54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3,13;-1</v>
       </c>
       <c r="X54" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6026,11 +6026,11 @@
       </c>
       <c r="AB54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>3,8;-1</v>
+        <v/>
       </c>
       <c r="AC54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>3,7;-1</v>
       </c>
       <c r="AD54" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="AE54" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>3,5;-1</v>
+        <v/>
       </c>
       <c r="AF54" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6071,9 +6071,6 @@
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E55" s="1" t="s">
         <v>1</v>
       </c>
@@ -6086,10 +6083,13 @@
       <c r="H55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M55" s="1" t="s">
@@ -6120,7 +6120,7 @@
       </c>
       <c r="W55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2,13;-1</v>
       </c>
       <c r="X55" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6140,11 +6140,11 @@
       </c>
       <c r="AB55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2,8;-1</v>
+        <v/>
       </c>
       <c r="AC55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>2,7;-1</v>
       </c>
       <c r="AD55" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6152,7 +6152,7 @@
       </c>
       <c r="AE55" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>2,5;-1</v>
+        <v/>
       </c>
       <c r="AF55" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6185,9 +6185,6 @@
       <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E56" s="1" t="s">
         <v>1</v>
       </c>
@@ -6200,10 +6197,13 @@
       <c r="H56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L56" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M56" s="1" t="s">
@@ -6234,7 +6234,7 @@
       </c>
       <c r="W56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1,13;-1</v>
       </c>
       <c r="X56" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6254,11 +6254,11 @@
       </c>
       <c r="AB56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1,8;-1</v>
+        <v/>
       </c>
       <c r="AC56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1,7;-1</v>
       </c>
       <c r="AD56" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="AE56" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>1,5;-1</v>
+        <v/>
       </c>
       <c r="AF56" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6299,9 +6299,6 @@
       <c r="C57" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E57" s="1" t="s">
         <v>1</v>
       </c>
@@ -6314,10 +6311,13 @@
       <c r="H57" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L57" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M57" s="1" t="s">
@@ -6348,7 +6348,7 @@
       </c>
       <c r="W57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0,13;-1</v>
       </c>
       <c r="X57" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6368,11 +6368,11 @@
       </c>
       <c r="AB57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0,8;-1</v>
+        <v/>
       </c>
       <c r="AC57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0,7;-1</v>
       </c>
       <c r="AD57" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6380,7 +6380,7 @@
       </c>
       <c r="AE57" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>0,5;-1</v>
+        <v/>
       </c>
       <c r="AF57" s="1" t="str">
         <f t="shared" si="5"/>

</xml_diff>